<commit_message>
Actualización semanal del ranking
</commit_message>
<xml_diff>
--- a/m_ranking Seghos 2025_26.xlsx
+++ b/m_ranking Seghos 2025_26.xlsx
@@ -464,16 +464,16 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="142" zoomScaleNormal="142" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="10.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
@@ -578,7 +578,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6" s="8" t="n">
         <v>2</v>
@@ -591,7 +591,7 @@
       </c>
       <c r="G6" s="10" t="n">
         <f aca="false">IF(C6="","",C6/B6)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>